<commit_message>
2020-10-24 Congratulation, Team IROS On-Demand
</commit_message>
<xml_diff>
--- a/polls/IROS20_Competition.xlsx
+++ b/polls/IROS20_Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akdba\Desktop\mysite\polls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4543306D-EAE3-457D-AB68-997C54B19849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CEE587-E26C-4546-91C8-83D3F9C17661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7C8864CB-4C3E-44E8-9D4C-0FA2FAE53705}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7C8864CB-4C3E-44E8-9D4C-0FA2FAE53705}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Nr</t>
   </si>
@@ -210,13 +210,31 @@
   </si>
   <si>
     <t>Video</t>
+  </si>
+  <si>
+    <t>October 20-23, 2020</t>
+  </si>
+  <si>
+    <t>Livestream presentation November 6, 2020 9-10:30am EST</t>
+  </si>
+  <si>
+    <t>The competition has two tracks: service robot track and manufacturing track. The service robot track has one simple task -- make five cups of iced Matcha green tea. There will be two manufacturing sub-tasks in the competition, disassembly and assembly using a NIST Task Board (NTB).</t>
+  </si>
+  <si>
+    <t>Corresponding Organizer</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>rahulm@seas.upenn.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +254,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -269,6 +294,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,22 +609,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA8EFFC8-626A-4E30-B826-7EEEED9D70E3}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:W4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="3" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
-    <col min="21" max="21" width="90" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="3" max="5" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.88671875" customWidth="1"/>
+    <col min="15" max="15" width="17" customWidth="1"/>
+    <col min="16" max="16" width="30.33203125" customWidth="1"/>
+    <col min="23" max="23" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1">
+    <row r="1" spans="1:23" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -618,52 +646,58 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -683,52 +717,58 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s">
         <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L2" t="s">
         <v>29</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
         <v>29</v>
       </c>
       <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q2" t="s">
         <v>26</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>27</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>31</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>28</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>32</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -738,44 +778,44 @@
       <c r="C3" t="s">
         <v>56</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>49</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>36</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>46</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>43</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>50</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>48</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>41</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>37</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>38</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -785,40 +825,52 @@
       <c r="C4" t="s">
         <v>44</v>
       </c>
-      <c r="G4" t="s">
+      <c r="E4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" t="s">
         <v>46</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>51</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>52</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>53</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>39</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>54</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>55</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" display="mailto:rahulm@seas.upenn.edu" xr:uid="{4D7D564B-283D-4A57-ADA2-44D6AA2347B6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>